<commit_message>
change startswith to include, edit data to use latin alphabet only
</commit_message>
<xml_diff>
--- a/OGHIST_2025_10_07.xlsx
+++ b/OGHIST_2025_10_07.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\GNIClassLookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C73E8A-D085-47AD-8CBE-41D0722DD3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1568B0-44E2-48CF-B0DA-6C6DDD0682B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="730" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14897" uniqueCount="969">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14897" uniqueCount="972">
   <si>
     <t>Document:</t>
   </si>
@@ -3116,6 +3116,15 @@
   </si>
   <si>
     <t>24</t>
+  </si>
+  <si>
+    <t>Sao Tome and Príncipe</t>
+  </si>
+  <si>
+    <t>Turkiye</t>
+  </si>
+  <si>
+    <t>Cote d'Ivoire</t>
   </si>
 </sst>
 </file>
@@ -6606,10 +6615,10 @@
   <dimension ref="A1:IS225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="3270" ySplit="495" topLeftCell="A32" activePane="bottomLeft"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A133" sqref="A133:XFD133"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <pane xSplit="3270" ySplit="495" activePane="bottomLeft"/>
+      <selection pane="topRight" activeCell="R1" sqref="R1:R1048576"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomRight" activeCell="A184" sqref="A184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12556,7 +12565,7 @@
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A49" s="44" t="s">
-        <v>306</v>
+        <v>971</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>548</v>
@@ -26598,7 +26607,7 @@
     </row>
     <row r="167" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A167" s="44" t="s">
-        <v>907</v>
+        <v>969</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>546</v>
@@ -30644,7 +30653,7 @@
     </row>
     <row r="201" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A201" s="44" t="s">
-        <v>908</v>
+        <v>970</v>
       </c>
       <c r="B201" s="3" t="s">
         <v>548</v>
@@ -54605,11 +54614,6 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
@@ -54617,31 +54621,14 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <i008215bacac45029ee8cafff4c8e93b xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DECDG - Development Data Group</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">2ae5ce6c-bf4c-4936-8a28-da4d57c09588</TermId>
-        </TermInfo>
-      </Terms>
-    </i008215bacac45029ee8cafff4c8e93b>
-    <Abstract xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-    <WBDocs_Access_To_Info_Exception xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">12. Not Assessed</WBDocs_Access_To_Info_Exception>
-    <TaxCatchAll xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Value>5</Value>
-    </TaxCatchAll>
-    <o1cb080a3dca4eb8a0fd03c7cc8bf8f7 xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </o1cb080a3dca4eb8a0fd03c7cc8bf8f7>
-    <OneCMS_Subcategory xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-    <WBDocs_Information_Classification xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">Official Use Only</WBDocs_Information_Classification>
-    <OneCMS_Category xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-    <WBDocs_Document_Date xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">2023-06-26T15:05:53+00:00</WBDocs_Document_Date>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="2a6c10d7-b926-4fc0-945e-3cbf5049f6bd" ContentTypeId="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F02" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -54887,11 +54874,41 @@
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="2a6c10d7-b926-4fc0-945e-3cbf5049f6bd" ContentTypeId="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F02" PreviousValue="false"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <i008215bacac45029ee8cafff4c8e93b xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DECDG - Development Data Group</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">2ae5ce6c-bf4c-4936-8a28-da4d57c09588</TermId>
+        </TermInfo>
+      </Terms>
+    </i008215bacac45029ee8cafff4c8e93b>
+    <Abstract xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+    <WBDocs_Access_To_Info_Exception xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">12. Not Assessed</WBDocs_Access_To_Info_Exception>
+    <TaxCatchAll xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Value>5</Value>
+    </TaxCatchAll>
+    <o1cb080a3dca4eb8a0fd03c7cc8bf8f7 xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </o1cb080a3dca4eb8a0fd03c7cc8bf8f7>
+    <OneCMS_Subcategory xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+    <WBDocs_Information_Classification xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">Official Use Only</WBDocs_Information_Classification>
+    <OneCMS_Category xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+    <WBDocs_Document_Date xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">2023-06-26T15:05:53+00:00</WBDocs_Document_Date>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F08796FC-F2AF-40F3-B2C0-0FC104661227}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DB51E32-A88A-4A12-90DD-F41DD2BB57BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -54899,20 +54916,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F08796FC-F2AF-40F3-B2C0-0FC104661227}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E0163D1-75F3-479B-97C7-B5428585AAD7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CA08370-99A5-4FA5-A2C3-E68D6DF39C51}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -54936,9 +54943,11 @@
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E0163D1-75F3-479B-97C7-B5428585AAD7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CA08370-99A5-4FA5-A2C3-E68D6DF39C51}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>